<commit_message>
Pivot tables created + updates
</commit_message>
<xml_diff>
--- a/sum_of_incidents_per_school_type_pivot_table.xlsx
+++ b/sum_of_incidents_per_school_type_pivot_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,38 +434,43 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>CHARTER SCH</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>ELEMENTARY</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>HIGH SCHOOL</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>MIDDLE SCHL</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t># of Discipline Incidents</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
         <v>4133</v>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>50045</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>125525</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>67177</v>
       </c>
     </row>

</xml_diff>